<commit_message>
fixed html and php slides
</commit_message>
<xml_diff>
--- a/articles.xlsx
+++ b/articles.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{DB773FF9-EEC0-4184-AEA2-198E0B9BE94A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{2C3193F9-C838-419A-B903-A9AEAD9BD4B2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="123">
   <si>
     <t>#</t>
   </si>
@@ -41,19 +41,373 @@
   </si>
   <si>
     <t>22/07/2018</t>
+  </si>
+  <si>
+    <t>Website Developer Roadmap</t>
+  </si>
+  <si>
+    <t>https://codeburst.io/the-2018-web-developer-roadmap-826b1b806e8d</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>Tags</t>
+  </si>
+  <si>
+    <t>Beginner</t>
+  </si>
+  <si>
+    <t>https://viblo.asia/p/cam-nang-cho-nguoi-bat-dau-hoc-lap-trinh-web-trong-nam-2018-WAyK8kG95xX</t>
+  </si>
+  <si>
+    <t>cẩm nang cho người bắt đầu học lập trình web trong năm 2018</t>
+  </si>
+  <si>
+    <t>https://viblo.asia/p/tim-hieu-ve-bem-gioi-thieu-qzaGzNMzGyO</t>
+  </si>
+  <si>
+    <t>Tìm hiểu về BEM - Giới thiệu</t>
+  </si>
+  <si>
+    <t>http://blog.appconus.com/2015/08/15/coding-conventions-trong-lap-trinh/</t>
+  </si>
+  <si>
+    <t>Coding conventions trong lập trình</t>
+  </si>
+  <si>
+    <t>https://webdesign.tutsplus.com/vi/tutorials/visual-studio-code-my-new-favorite-code-editor--cms-28012</t>
+  </si>
+  <si>
+    <t>Visual Studio Code: Code Editor yêu thích mới của tôi</t>
+  </si>
+  <si>
+    <t>https://viblo.asia/p/8-visual-studio-code-extensions-huu-ich-danh-cho-front-end-developer-gGJ59XQplX2</t>
+  </si>
+  <si>
+    <t>8 Visual Studio Code Extensions hữu ích dành cho Front End Developer</t>
+  </si>
+  <si>
+    <t>https://viblo.asia/p/gioi-thieu-ve-visual-studio-code-DXOkRZaBkdZ</t>
+  </si>
+  <si>
+    <t>Giới thiệu về Visual Studio Code</t>
+  </si>
+  <si>
+    <t>https://vscodecandothat.com/</t>
+  </si>
+  <si>
+    <t>VS Code can do that?!</t>
+  </si>
+  <si>
+    <t>https://kipalog.com/posts/Lap-trinh-vien-co-can-gioi-Tieng-Anh</t>
+  </si>
+  <si>
+    <t>Lập trình viên có cần giỏi Tiếng Anh</t>
+  </si>
+  <si>
+    <t>http://itcviet.com/viet-code-nhanh-hon-voi-emmet-plugin/</t>
+  </si>
+  <si>
+    <t>Viết code nhanh hơn với Emmet plugin</t>
+  </si>
+  <si>
+    <t>https://aptech-danang.edu.vn/ace/tin-tuc-su-kien/chi-tiet/16544/cac-phan-mo-rong-vscode-javascript-hang-dau-de-phat-trien-nhanh-hon</t>
+  </si>
+  <si>
+    <t>CÁC PHẦN MỞ RỘNG VSCODE JAVASCRIPT HÀNG ĐẦU ĐỂ PHÁT TRIỂN NHANH HƠN</t>
+  </si>
+  <si>
+    <t>https://viblo.asia/p/tim-hieu-the-gioi-web-tu-con-so-0-part-i-web-server-EyORkbEEGqB</t>
+  </si>
+  <si>
+    <t>Tìm hiểu thế giới web từ con số 0 (Part I)- Web server</t>
+  </si>
+  <si>
+    <t>https://gist.github.com/poopsplat/7195274</t>
+  </si>
+  <si>
+    <t>https://viblo.asia/p/nhung-lenh-git-co-ban-can-nho-V3m5W1OyZO7</t>
+  </si>
+  <si>
+    <t>Những lệnh Git cơ bản cần nhớ</t>
+  </si>
+  <si>
+    <t>https://viblo.asia/p/su-dung-sass-de-viet-css-chuyen-nghiep-va-hieu-qua-PDOkqMKDkjx</t>
+  </si>
+  <si>
+    <t>Sử dụng SASS để viết CSS chuyên nghiệp và hiệu quả</t>
+  </si>
+  <si>
+    <t>https://nguyenhuuhoang.com/huong-dan-cai-dat-ubuntu-16-04-desktop-bang-usb/</t>
+  </si>
+  <si>
+    <t>Hướng dẫn cài đặt Ubuntu 16.04 Desktop bằng usb</t>
+  </si>
+  <si>
+    <t>https://chiasefree.com/linux-tutorials/huong-dan-cai-ubuntu-16-04</t>
+  </si>
+  <si>
+    <t>Hướng dẫn cài Ubuntu 16.04 song song với windows 7, 8,10</t>
+  </si>
+  <si>
+    <t>https://toidicode.com/lamp-la-gi-177.html</t>
+  </si>
+  <si>
+    <t>LAMP là gì?</t>
+  </si>
+  <si>
+    <t>https://kipalog.com/posts/Huong-dan-cai-dat-LAMP-tren-Ubuntu-16-04</t>
+  </si>
+  <si>
+    <t>Hướng dẫn cài đặt LAMP trên Ubuntu 16.04</t>
+  </si>
+  <si>
+    <t>https://kipalog.com/posts/Can-lam-nhung-gi-truoc--trong-va-sau-khi-cai-dat-Ubuntu</t>
+  </si>
+  <si>
+    <t>Cần làm những gì trước, trong và sau khi cài đặt Ubuntu</t>
+  </si>
+  <si>
+    <t>https://viblo.asia/p/php-10-loi-pho-bien-ma-cac-lap-trinh-vien-php-thuong-mac-phai-phan-1-yMnKMqmmK7P</t>
+  </si>
+  <si>
+    <t>PHP - 10 lỗi phổ biến mà các lập trình viên PHP thường mắc phải (Phần 1)</t>
+  </si>
+  <si>
+    <t>https://viblo.asia/p/series-php-lap-trinh-huong-doi-tuong-phan-1-GrLZDbzO5k0</t>
+  </si>
+  <si>
+    <t>Series PHP - Lập trình hướng đối tượng (Phần 1)</t>
+  </si>
+  <si>
+    <t>https://viblo.asia/p/tim-hieu-ve-he-thong-quan-li-co-so-du-lieu-mysql-3ZabG91oGzY6</t>
+  </si>
+  <si>
+    <t>Tìm hiểu về hệ thống quản lí cơ sở dữ liệu MySQL</t>
+  </si>
+  <si>
+    <t>https://kipalog.com/posts/4-tinh-chat-dac-thu-cua-lap-trinh-huong-doi-tuong</t>
+  </si>
+  <si>
+    <t>4 tính chất đặc thù của lập trình hướng đối tượng</t>
+  </si>
+  <si>
+    <t>https://viblo.asia/p/freecodecamp-la-gi-aWj538zwK6m</t>
+  </si>
+  <si>
+    <t>FreeCodeCamp là gì ?</t>
+  </si>
+  <si>
+    <t>https://techtalk.vn/tai-sao-cac-developer-nen-hoc-command-line.html</t>
+  </si>
+  <si>
+    <t>TẠI SAO CÁC DEVELOPER NÊN HỌC COMMAND LINE</t>
+  </si>
+  <si>
+    <t>https://techmaster.vn/posts/33903/giai-thich-ve-mo-hinh-mvc</t>
+  </si>
+  <si>
+    <t>Đi uống nước mía học về MVC</t>
+  </si>
+  <si>
+    <t>https://lmt.com.vn/php/tim-hieu-php/360-tim-hieu-mo-hinh-mvc-la-gi.html</t>
+  </si>
+  <si>
+    <t>Tìm hiểu mô hình MVC là gì ?</t>
+  </si>
+  <si>
+    <t>https://viblo.asia/p/cai-dat-ung-dung-php-thuan-su-dung-mvc-va-oop-4P856aA3lY3</t>
+  </si>
+  <si>
+    <t>Cài đặt ứng dụng PHP thuần sử dụng MVC và OOP</t>
+  </si>
+  <si>
+    <t>https://viblo.asia/p/tim-hieu-laravel-tu-so-0-rQOvPKlNkYj</t>
+  </si>
+  <si>
+    <t>Tìm hiểu Laravel từ số 0</t>
+  </si>
+  <si>
+    <t>https://aptech-danang.edu.vn/ace/tin-tuc-su-kien/chi-tiet/16517/tong-hop-cac-text-editor-dinh-cho-dan-coder</t>
+  </si>
+  <si>
+    <t>TỔNG HỢP CÁC TEXT EDITOR "ĐỈNH" CHO DÂN CODER</t>
+  </si>
+  <si>
+    <t>https://viblo.asia/p/tim-hieu-laravel-tu-so-0-p2-XQZGxojovwA</t>
+  </si>
+  <si>
+    <t>Tìm hiểu Laravel từ số 0 (P2) - View</t>
+  </si>
+  <si>
+    <t>https://letsclearitup.com.ua/books/2017/laravel_5_cookbook.pdf</t>
+  </si>
+  <si>
+    <t>Laravel Cookbook</t>
+  </si>
+  <si>
+    <t>https://viblo.asia/p/co-ban-ve-routing-trong-laravel-qzakzLoOGyO</t>
+  </si>
+  <si>
+    <t>Cơ bản về Routing trong Laravel</t>
+  </si>
+  <si>
+    <t>https://itsolutionstuff.com/post/laravel-55-crud-example-from-scratchexample.html</t>
+  </si>
+  <si>
+    <t>Laravel 5.5 CRUD Example from scratch</t>
+  </si>
+  <si>
+    <t>https://appdividend.com/2017/10/15/laravel-5-5-crud-example-tutorial/</t>
+  </si>
+  <si>
+    <t>Laravel 5.5 CRUD Tutorial Example Step By Step From Scratch</t>
+  </si>
+  <si>
+    <t>https://viblo.asia/p/migration-va-seeder-L4x5xgDalBM</t>
+  </si>
+  <si>
+    <t>Migration và Seeder</t>
+  </si>
+  <si>
+    <t>https://toidicode.com/model-trong-laravel-12.html</t>
+  </si>
+  <si>
+    <t>Model trong Laravel</t>
+  </si>
+  <si>
+    <t>https://allaravel.com/laravel-tutorials/laravel-migration-va-laravel-seeding-quan-ly-phien-ban-database/</t>
+  </si>
+  <si>
+    <t>Laravel Migration và Laravel Seeding: quản lý phiên bản database</t>
+  </si>
+  <si>
+    <t>https://uxplanet.org/how-the-bootstrap-4-grid-works-a1b04703a3b7</t>
+  </si>
+  <si>
+    <t>How the Bootstrap 4 Grid Works</t>
+  </si>
+  <si>
+    <t>https://viblo.asia/p/huong-nghiep-trong-nganh-cong-nghe-thong-tin-Qpmle9kVlrd</t>
+  </si>
+  <si>
+    <t>Hướng nghiệp trong ngành công nghệ thông tin</t>
+  </si>
+  <si>
+    <t>https://medium.freecodecamp.org/the-absolute-beginners-guide-to-learning-web-development-in-2018-d87ba925549b</t>
+  </si>
+  <si>
+    <t>The absolute beginner’s guide to learning web development in 2018</t>
+  </si>
+  <si>
+    <t>Command Line trên Mac, tương tự như trên Git Bash</t>
+  </si>
+  <si>
+    <t>https://thachpham.com/tools/git-git-va-github-la-gi-tai-sao-nen-dung.html</t>
+  </si>
+  <si>
+    <t>[GIT] GIT VÀ GITHUB LÀ GÌ? TẠI SAO NÊN DÙNG?</t>
+  </si>
+  <si>
+    <t>https://www.topitworks.com/blogs/freecodecamp/</t>
+  </si>
+  <si>
+    <t>Từ con số 0 tôi đã trở thành lập trình viên trong vòng 12 tháng như thế nào?</t>
+  </si>
+  <si>
+    <t>https://viblo.asia/p/lo-trinh-tro-thanh-lap-trinh-vien-front-end-2018-Az45bnBL5xY</t>
+  </si>
+  <si>
+    <t>LỘ TRÌNH TRỞ THÀNH LẬP TRÌNH VIÊN FRONT-END 2018</t>
+  </si>
+  <si>
+    <t>https://viblo.asia/p/css-cho-nguoi-moi-bat-dau-gDVK28NvlLj</t>
+  </si>
+  <si>
+    <t>Css cho người mới bắt đầu</t>
+  </si>
+  <si>
+    <t>https://kipalog.com/posts/Bootstrap-la-gi--Gioi-thieu-ve-bootstrap-va-hoc-bootstrap--bootstrap-tutorial</t>
+  </si>
+  <si>
+    <t>Bootstrap là gì? Giới thiệu về bootstrap và học bootstrap, bootstrap tutorial</t>
+  </si>
+  <si>
+    <t>https://freetuts.net/hoc-git/github-can-ban-va-nang-cao</t>
+  </si>
+  <si>
+    <t>Github căn bản và nâng cao | Github là gì?</t>
+  </si>
+  <si>
+    <t>https://thachpham.com/web-development/html-css/html-va-css-can-ban-danh-cho-cho-moi-nguoi.html</t>
+  </si>
+  <si>
+    <t>HTML VÀ CSS CĂN BẢN DÀNH CHO CHO MỌI NGƯỜI</t>
+  </si>
+  <si>
+    <t>https://viblo.asia/p/bai-2-tim-hieu-ve-grid-system-trong-bootstrap-MgNeWXjRkYx</t>
+  </si>
+  <si>
+    <t>Tìm hiểu về Grid System trong Bootstrap</t>
+  </si>
+  <si>
+    <t>https://dancongngheorg.wordpress.com/2018/03/20/tim-hieu-bootstrap-4-trong-5-phut/</t>
+  </si>
+  <si>
+    <t>Tìm hiểu Bootstrap 4 trong 5 phút</t>
+  </si>
+  <si>
+    <t>https://techmaster.vn/posts/34637/nhung-extension-duoc-yeu-thich-nhat-nam-2017-cua-visual-studio-code</t>
+  </si>
+  <si>
+    <t>Những extension được yêu thích nhất năm 2017 của Visual Studio Code</t>
+  </si>
+  <si>
+    <t>https://viblo.asia/p/gioi-thieu-ve-media-css-trong-responsive-4dbZNDEL5YM</t>
+  </si>
+  <si>
+    <t>Giới thiệu về Media CSS trong Responsive</t>
+  </si>
+  <si>
+    <t>https://viblo.asia/p/bat-dau-voi-javascript-p1-XL6lAgnNKek</t>
+  </si>
+  <si>
+    <t>Bắt Đầu với Javascript (P1)</t>
+  </si>
+  <si>
+    <t>https://viblo.asia/p/phan-biet-giua-front-end-back-end-va-full-stack-WAyK8RGnlxX</t>
+  </si>
+  <si>
+    <t>Phân biệt giữa Front End, Back End và Full Stack</t>
+  </si>
+  <si>
+    <t>https://vinasupport.com/tong-hop-extension-nen-dung-cho-visual-studio-code/</t>
+  </si>
+  <si>
+    <t>Tổng hợp Extension nên dùng cho Visual Studio Code</t>
+  </si>
+  <si>
+    <t>29/07/2018</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1D2129"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -76,8 +430,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -358,15 +714,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:D3"/>
+  <dimension ref="A2:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C31" activeCellId="1" sqref="B31 C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="36.140625" customWidth="1"/>
+    <col min="3" max="3" width="64.85546875" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" customWidth="1"/>
+    <col min="5" max="5" width="21" customWidth="1"/>
+    <col min="6" max="6" width="31.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -377,21 +740,818 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>43</v>
+      </c>
       <c r="B3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>56</v>
+      </c>
+      <c r="B4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C4" t="s">
+        <v>118</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>46</v>
+      </c>
+      <c r="B5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>44</v>
+      </c>
+      <c r="B9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C9" t="s">
+        <v>94</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C10" t="s">
         <v>4</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F10" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C12" t="s">
+        <v>91</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>7</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>8</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>9</v>
+      </c>
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>10</v>
+      </c>
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>12</v>
+      </c>
+      <c r="B19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>13</v>
+      </c>
+      <c r="B20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>14</v>
+      </c>
+      <c r="B21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" t="s">
+        <v>32</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>15</v>
+      </c>
+      <c r="B22" t="s">
+        <v>93</v>
+      </c>
+      <c r="C22" t="s">
+        <v>34</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>17</v>
+      </c>
+      <c r="B23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" t="s">
+        <v>37</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>18</v>
+      </c>
+      <c r="B24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" t="s">
+        <v>39</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>19</v>
+      </c>
+      <c r="B25" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" t="s">
+        <v>41</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>20</v>
+      </c>
+      <c r="B26" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>21</v>
+      </c>
+      <c r="B27" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" t="s">
+        <v>45</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>22</v>
+      </c>
+      <c r="B28" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>23</v>
+      </c>
+      <c r="B29" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" t="s">
+        <v>49</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>24</v>
+      </c>
+      <c r="B30" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" t="s">
+        <v>51</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>25</v>
+      </c>
+      <c r="B31" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" t="s">
+        <v>53</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>26</v>
+      </c>
+      <c r="B32" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" t="s">
+        <v>55</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>27</v>
+      </c>
+      <c r="B33" t="s">
+        <v>58</v>
+      </c>
+      <c r="C33" t="s">
+        <v>57</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>28</v>
+      </c>
+      <c r="B34" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" t="s">
+        <v>59</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>29</v>
+      </c>
+      <c r="B35" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35" t="s">
+        <v>61</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>30</v>
+      </c>
+      <c r="B36" t="s">
+        <v>64</v>
+      </c>
+      <c r="C36" t="s">
+        <v>63</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>31</v>
+      </c>
+      <c r="B37" t="s">
+        <v>66</v>
+      </c>
+      <c r="C37" t="s">
+        <v>65</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>32</v>
+      </c>
+      <c r="B38" t="s">
+        <v>68</v>
+      </c>
+      <c r="C38" t="s">
+        <v>67</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>33</v>
+      </c>
+      <c r="B39" t="s">
+        <v>70</v>
+      </c>
+      <c r="C39" t="s">
+        <v>69</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>34</v>
+      </c>
+      <c r="B40" t="s">
+        <v>72</v>
+      </c>
+      <c r="C40" t="s">
+        <v>71</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>35</v>
+      </c>
+      <c r="B41" t="s">
+        <v>74</v>
+      </c>
+      <c r="C41" t="s">
+        <v>73</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>36</v>
+      </c>
+      <c r="B42" t="s">
+        <v>76</v>
+      </c>
+      <c r="C42" t="s">
+        <v>75</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>37</v>
+      </c>
+      <c r="B43" t="s">
+        <v>78</v>
+      </c>
+      <c r="C43" t="s">
+        <v>77</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>38</v>
+      </c>
+      <c r="B44" t="s">
+        <v>80</v>
+      </c>
+      <c r="C44" t="s">
+        <v>79</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>39</v>
+      </c>
+      <c r="B45" t="s">
+        <v>82</v>
+      </c>
+      <c r="C45" t="s">
+        <v>81</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>40</v>
+      </c>
+      <c r="B46" t="s">
+        <v>84</v>
+      </c>
+      <c r="C46" t="s">
+        <v>83</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>41</v>
+      </c>
+      <c r="B47" t="s">
+        <v>86</v>
+      </c>
+      <c r="C47" t="s">
+        <v>85</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>42</v>
+      </c>
+      <c r="B48" t="s">
+        <v>88</v>
+      </c>
+      <c r="C48" t="s">
+        <v>87</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>45</v>
+      </c>
+      <c r="B49" t="s">
+        <v>97</v>
+      </c>
+      <c r="C49" t="s">
+        <v>96</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>47</v>
+      </c>
+      <c r="B50" t="s">
+        <v>101</v>
+      </c>
+      <c r="C50" t="s">
+        <v>100</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>48</v>
+      </c>
+      <c r="B51" t="s">
+        <v>103</v>
+      </c>
+      <c r="C51" t="s">
+        <v>102</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>49</v>
+      </c>
+      <c r="B52" t="s">
+        <v>105</v>
+      </c>
+      <c r="C52" t="s">
+        <v>104</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>50</v>
+      </c>
+      <c r="B53" t="s">
+        <v>107</v>
+      </c>
+      <c r="C53" t="s">
+        <v>106</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>51</v>
+      </c>
+      <c r="B54" t="s">
+        <v>109</v>
+      </c>
+      <c r="C54" t="s">
+        <v>108</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>52</v>
+      </c>
+      <c r="B55" t="s">
+        <v>111</v>
+      </c>
+      <c r="C55" t="s">
+        <v>110</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>53</v>
+      </c>
+      <c r="B56" t="s">
+        <v>113</v>
+      </c>
+      <c r="C56" t="s">
+        <v>112</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>54</v>
+      </c>
+      <c r="B57" t="s">
+        <v>115</v>
+      </c>
+      <c r="C57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>55</v>
+      </c>
+      <c r="B58" t="s">
+        <v>117</v>
+      </c>
+      <c r="C58" t="s">
+        <v>116</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>57</v>
+      </c>
+      <c r="B59" t="s">
+        <v>121</v>
+      </c>
+      <c r="C59" t="s">
+        <v>120</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>